<commit_message>
Please add this new change commit
</commit_message>
<xml_diff>
--- a/Config/Bug_Check.xlsx
+++ b/Config/Bug_Check.xlsx
@@ -1,51 +1,96 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jnj-my.sharepoint.com/personal/praj7_its_jnj_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRaj7\PycharmProjects\DORUserStory\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{286F5580-6786-4B2C-AB57-88D975904D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034A747F-F801-4FCE-A2E4-F737BD2CAF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19100" windowHeight="9020" xr2:uid="{15E3E94D-FD87-4E30-97CE-819A18BE76C3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="URL" sheetId="1" r:id="rId1"/>
+    <sheet name="Result" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
   <si>
     <t>JIRA ID</t>
+  </si>
+  <si>
+    <t>https://jira.jnj.com/browse/AGQP-293</t>
+  </si>
+  <si>
+    <t>https://jira.jnj.com/browse/AGQP-294</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Epic</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Affected Version</t>
+  </si>
+  <si>
+    <t>Fix Version</t>
+  </si>
+  <si>
+    <t>Story Point</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Approval Workflow</t>
+  </si>
+  <si>
+    <t>Asignee/Reporter</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Update the type as Story</t>
+  </si>
+  <si>
+    <t>Add the Story Point</t>
+  </si>
+  <si>
+    <t>Add the acceptance criteria</t>
+  </si>
+  <si>
+    <t>Assignee/Reporter Cant be Same</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,13 +98,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -71,13 +136,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -409,24 +479,174 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60E3D0D-C016-4D68-8181-56A0692BCE3D}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>